<commit_message>
add device.xlsx init into database/add device v2
</commit_message>
<xml_diff>
--- a/runtime/export/device.xlsx
+++ b/runtime/export/device.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17448" windowHeight="8375"/>
+    <workbookView windowWidth="21288" windowHeight="10535" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="设备基本信息表" sheetId="1" r:id="rId1"/>
     <sheet name="设备类型代码表" sheetId="2" r:id="rId2"/>
     <sheet name="设备状态代码表" sheetId="3" r:id="rId3"/>
+    <sheet name="操作类型代码表" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
   <si>
     <t>资产编号</t>
   </si>
@@ -123,24 +124,30 @@
     <t>名称</t>
   </si>
   <si>
-    <t>dyj</t>
+    <t>DYJ</t>
   </si>
   <si>
     <t>打印机</t>
   </si>
   <si>
-    <t>jsj1</t>
+    <t>JSJ</t>
   </si>
   <si>
     <t>计算机</t>
   </si>
   <si>
-    <t>wl</t>
+    <t>JHJ</t>
   </si>
   <si>
     <t>交换机</t>
   </si>
   <si>
+    <t>LYQ</t>
+  </si>
+  <si>
+    <t>路由器</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -181,6 +188,18 @@
   </si>
   <si>
     <t>已调离（不在市局管理范围）</t>
+  </si>
+  <si>
+    <t>分发</t>
+  </si>
+  <si>
+    <t>回收</t>
+  </si>
+  <si>
+    <t>报废</t>
+  </si>
+  <si>
+    <t>借调</t>
   </si>
 </sst>
 </file>
@@ -189,9 +208,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -362,36 +381,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -410,42 +429,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -458,91 +477,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,129 +680,138 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -791,15 +819,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1158,7 +1177,7 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1246,13 +1265,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1284,6 +1303,14 @@
       </c>
       <c r="B4" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1299,7 +1326,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A1" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="1"/>
@@ -1317,58 +1344,58 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1376,4 +1403,64 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="38.8888888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add device new version
</commit_message>
<xml_diff>
--- a/runtime/export/device.xlsx
+++ b/runtime/export/device.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21288" windowHeight="10535" activeTab="3"/>
+    <workbookView windowWidth="21288" windowHeight="11484" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="设备基本信息表" sheetId="1" r:id="rId1"/>
     <sheet name="设备类型代码表" sheetId="2" r:id="rId2"/>
     <sheet name="设备状态代码表" sheetId="3" r:id="rId3"/>
     <sheet name="操作类型代码表" sheetId="4" r:id="rId4"/>
+    <sheet name="设备属性代码表" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
   <si>
     <t>资产编号</t>
   </si>
@@ -103,7 +104,7 @@
     <t>供应商</t>
   </si>
   <si>
-    <t>设备状态</t>
+    <t>设备状态（新版无此列）</t>
   </si>
   <si>
     <t>请参照设备类型代码表</t>
@@ -151,55 +152,85 @@
     <t>1</t>
   </si>
   <si>
-    <t>个人在用</t>
+    <t>在库</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>科室公用</t>
+    <t>在用</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>待分配（存信息中心、可分配）</t>
+    <t>借用</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>已借用（属信息中心、其他科室借用）</t>
+    <t>在途</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>不可用（已坏未报废）</t>
+    <t>报废</t>
+  </si>
+  <si>
+    <t>设备入库</t>
+  </si>
+  <si>
+    <t>设备出库</t>
+  </si>
+  <si>
+    <t>分配共用</t>
+  </si>
+  <si>
+    <t>分配专有</t>
+  </si>
+  <si>
+    <t>借出共用</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>已报废（收回至信息中心）</t>
+    <t>借出专有</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>已调离（不在市局管理范围）</t>
-  </si>
-  <si>
-    <t>分发</t>
-  </si>
-  <si>
-    <t>回收</t>
-  </si>
-  <si>
-    <t>报废</t>
-  </si>
-  <si>
-    <t>借调</t>
+    <t>设备收回</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>设备交回</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>设备报废</t>
+  </si>
+  <si>
+    <t>在库设备</t>
+  </si>
+  <si>
+    <t>在途设备</t>
+  </si>
+  <si>
+    <t>共用设备</t>
+  </si>
+  <si>
+    <t>专有设备</t>
+  </si>
+  <si>
+    <t>报废设备</t>
   </si>
 </sst>
 </file>
@@ -207,9 +238,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -228,6 +259,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -240,6 +279,89 @@
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -251,16 +373,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,98 +390,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,19 +418,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,157 +592,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -586,6 +617,36 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,17 +675,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -639,39 +703,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -680,10 +711,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -692,133 +723,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1178,7 +1209,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1323,15 +1354,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="2" max="2" width="38.8888888888889" customWidth="1"/>
+    <col min="1" max="2" width="5.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1382,21 +1413,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1408,15 +1435,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="2" max="2" width="38.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="9.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1432,7 +1460,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1440,7 +1468,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1448,7 +1476,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1456,8 +1484,129 @@
         <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="5.66666666666667" customWidth="1"/>
+    <col min="2" max="2" width="9.66666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>